<commit_message>
Fixing  test machine excel files
</commit_message>
<xml_diff>
--- a/inst/extdata/Machines - Data/Automobiles/Automobiles.xlsx
+++ b/inst/extdata/Machines - Data/Automobiles/Automobiles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Country</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Final</t>
-  </si>
-  <si>
-    <t>FInal</t>
   </si>
   <si>
     <t>PCM</t>
@@ -523,7 +520,7 @@
   <dimension ref="A1:BI53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,16 +582,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="7">
         <v>0.3</v>
@@ -666,16 +663,16 @@
         <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
@@ -692,19 +689,19 @@
         <v>18</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="H5" s="7">
         <v>0.3</v>
@@ -721,19 +718,19 @@
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
@@ -1012,18 +1009,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,14 +1043,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF083C1D-CE62-48EF-BAF9-9D27C80F6E5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1068,4 +1057,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>